<commit_message>
Fix sidebar profile section
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -37,13 +37,22 @@
     <t>kamanda@gmail.com</t>
   </si>
   <si>
-    <t>$2a$10$o240k1//7UDhGfpV20PwueDqqnwDoD.Qsw9rSkdB7lc.6jFkqMgCG</t>
+    <t>$2a$10$Bz4/5bkmPGFx.KNDLW2Us.iO2Q9dDQjt0wGkqqVFHyeLfHTjb.EF.</t>
   </si>
   <si>
     <t>agent</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>M'mah Zombo</t>
+  </si>
+  <si>
+    <t>zombo@gmail.com</t>
+  </si>
+  <si>
+    <t>$2a$10$/sNF3JT9o2N3GlJj//AFE.bxtu9fT9CyTXrZD1iaVRM9g9nH8UaCa</t>
   </si>
 </sst>
 </file>
@@ -420,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,6 +469,26 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>